<commit_message>
run 5 done for span 10
</commit_message>
<xml_diff>
--- a/series_02/mpi_0/span_010/qsmf_output.xlsx
+++ b/series_02/mpi_0/span_010/qsmf_output.xlsx
@@ -395,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2275,13 +2275,13 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73">
-        <v>-9</v>
+        <v>2</v>
       </c>
       <c r="B73">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C73">
-        <v>4.6033</v>
+        <v>-1.4611</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -2301,13 +2301,13 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="B74">
         <v>6</v>
       </c>
       <c r="C74">
-        <v>5.2784</v>
+        <v>4.6033</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -2327,13 +2327,13 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="B75">
         <v>6</v>
       </c>
       <c r="C75">
-        <v>5.8279</v>
+        <v>5.2784</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -2353,13 +2353,13 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="B76">
         <v>6</v>
       </c>
       <c r="C76">
-        <v>6.3401</v>
+        <v>5.8279</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -2379,13 +2379,13 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="B77">
         <v>6</v>
       </c>
       <c r="C77">
-        <v>6.6346</v>
+        <v>6.3401</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2405,13 +2405,13 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="B78">
         <v>6</v>
       </c>
       <c r="C78">
-        <v>6.7814</v>
+        <v>6.6346</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -2431,13 +2431,13 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="B79">
         <v>6</v>
       </c>
       <c r="C79">
-        <v>6.4291</v>
+        <v>6.7814</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -2457,13 +2457,13 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B80">
         <v>6</v>
       </c>
       <c r="C80">
-        <v>5.3739</v>
+        <v>6.4291</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -2483,13 +2483,13 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="B81">
         <v>6</v>
       </c>
       <c r="C81">
-        <v>3.2795</v>
+        <v>5.3739</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2509,13 +2509,13 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82">
-        <v>-8</v>
+        <v>-1</v>
       </c>
       <c r="B82">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C82">
-        <v>5.1638</v>
+        <v>5.1433</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -2535,13 +2535,13 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83">
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="B83">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C83">
-        <v>5.7085</v>
+        <v>3.2795</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -2561,13 +2561,13 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84">
-        <v>-6</v>
+        <v>1</v>
       </c>
       <c r="B84">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C84">
-        <v>6.2424</v>
+        <v>0.64904</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -2587,13 +2587,13 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="B85">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C85">
-        <v>6.5467</v>
+        <v>-2.2381</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -2613,13 +2613,13 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86">
-        <v>-4</v>
+        <v>-9</v>
       </c>
       <c r="B86">
         <v>7</v>
       </c>
       <c r="C86">
-        <v>6.7052</v>
+        <v>4.5494</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -2639,13 +2639,13 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87">
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="B87">
         <v>7</v>
       </c>
       <c r="C87">
-        <v>6.5723</v>
+        <v>5.1638</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -2665,13 +2665,13 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88">
-        <v>-1</v>
+        <v>-7</v>
       </c>
       <c r="B88">
         <v>7</v>
       </c>
       <c r="C88">
-        <v>5.1051</v>
+        <v>5.7085</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -2691,13 +2691,13 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89">
-        <v>1</v>
+        <v>-6</v>
       </c>
       <c r="B89">
         <v>7</v>
       </c>
       <c r="C89">
-        <v>2.2049</v>
+        <v>6.2424</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -2717,13 +2717,13 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90">
-        <v>-9</v>
+        <v>-5</v>
       </c>
       <c r="B90">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C90">
-        <v>4.44</v>
+        <v>6.5467</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -2743,13 +2743,13 @@
     </row>
     <row r="91" spans="1:8">
       <c r="A91">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="B91">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C91">
-        <v>6.4409</v>
+        <v>6.7052</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -2772,10 +2772,10 @@
         <v>-3</v>
       </c>
       <c r="B92">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C92">
-        <v>6.7729</v>
+        <v>6.5723</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -2798,10 +2798,10 @@
         <v>-2</v>
       </c>
       <c r="B93">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C93">
-        <v>6.5031</v>
+        <v>5.7703</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -2824,10 +2824,10 @@
         <v>-1</v>
       </c>
       <c r="B94">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C94">
-        <v>5.6733</v>
+        <v>5.1051</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -2847,13 +2847,13 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95">
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="B95">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C95">
-        <v>4.9098</v>
+        <v>3.7594</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -2873,13 +2873,13 @@
     </row>
     <row r="96" spans="1:8">
       <c r="A96">
-        <v>-7</v>
+        <v>1</v>
       </c>
       <c r="B96">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C96">
-        <v>5.4203</v>
+        <v>2.2049</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -2899,13 +2899,13 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97">
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="B97">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C97">
-        <v>6.6888</v>
+        <v>-0.62087</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -2925,13 +2925,13 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="B98">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C98">
-        <v>6.8123</v>
+        <v>4.5279</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -2951,27 +2951,495 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99">
+        <v>-8</v>
+      </c>
+      <c r="B99">
+        <v>8</v>
+      </c>
+      <c r="C99">
+        <v>5.0744</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>250</v>
+      </c>
+      <c r="F99">
+        <v>112</v>
+      </c>
+      <c r="G99">
+        <v>0.16</v>
+      </c>
+      <c r="H99">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100">
+        <v>-7</v>
+      </c>
+      <c r="B100">
+        <v>8</v>
+      </c>
+      <c r="C100">
+        <v>5.5962</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>250</v>
+      </c>
+      <c r="F100">
+        <v>112</v>
+      </c>
+      <c r="G100">
+        <v>0.16</v>
+      </c>
+      <c r="H100">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101">
+        <v>-6</v>
+      </c>
+      <c r="B101">
+        <v>8</v>
+      </c>
+      <c r="C101">
+        <v>6.1046</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>250</v>
+      </c>
+      <c r="F101">
+        <v>112</v>
+      </c>
+      <c r="G101">
+        <v>0.16</v>
+      </c>
+      <c r="H101">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102">
+        <v>-5</v>
+      </c>
+      <c r="B102">
+        <v>8</v>
+      </c>
+      <c r="C102">
+        <v>6.5001</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>250</v>
+      </c>
+      <c r="F102">
+        <v>112</v>
+      </c>
+      <c r="G102">
+        <v>0.16</v>
+      </c>
+      <c r="H102">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103">
+        <v>-3</v>
+      </c>
+      <c r="B103">
+        <v>8</v>
+      </c>
+      <c r="C103">
+        <v>6.7209</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>250</v>
+      </c>
+      <c r="F103">
+        <v>112</v>
+      </c>
+      <c r="G103">
+        <v>0.16</v>
+      </c>
+      <c r="H103">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104">
+        <v>-2</v>
+      </c>
+      <c r="B104">
+        <v>8</v>
+      </c>
+      <c r="C104">
+        <v>6.3868</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>250</v>
+      </c>
+      <c r="F104">
+        <v>112</v>
+      </c>
+      <c r="G104">
+        <v>0.16</v>
+      </c>
+      <c r="H104">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105">
+        <v>8</v>
+      </c>
+      <c r="C105">
+        <v>1.7325</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>250</v>
+      </c>
+      <c r="F105">
+        <v>112</v>
+      </c>
+      <c r="G105">
+        <v>0.16</v>
+      </c>
+      <c r="H105">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106">
+        <v>-9</v>
+      </c>
+      <c r="B106">
+        <v>9</v>
+      </c>
+      <c r="C106">
+        <v>4.44</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>250</v>
+      </c>
+      <c r="F106">
+        <v>112</v>
+      </c>
+      <c r="G106">
+        <v>0.16</v>
+      </c>
+      <c r="H106">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107">
+        <v>-5</v>
+      </c>
+      <c r="B107">
+        <v>9</v>
+      </c>
+      <c r="C107">
+        <v>6.4409</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>250</v>
+      </c>
+      <c r="F107">
+        <v>112</v>
+      </c>
+      <c r="G107">
+        <v>0.16</v>
+      </c>
+      <c r="H107">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108">
+        <v>-3</v>
+      </c>
+      <c r="B108">
+        <v>9</v>
+      </c>
+      <c r="C108">
+        <v>6.7729</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>250</v>
+      </c>
+      <c r="F108">
+        <v>112</v>
+      </c>
+      <c r="G108">
+        <v>0.16</v>
+      </c>
+      <c r="H108">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109">
+        <v>-2</v>
+      </c>
+      <c r="B109">
+        <v>9</v>
+      </c>
+      <c r="C109">
+        <v>6.5031</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>250</v>
+      </c>
+      <c r="F109">
+        <v>112</v>
+      </c>
+      <c r="G109">
+        <v>0.16</v>
+      </c>
+      <c r="H109">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110">
+        <v>-1</v>
+      </c>
+      <c r="B110">
+        <v>9</v>
+      </c>
+      <c r="C110">
+        <v>5.6733</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>250</v>
+      </c>
+      <c r="F110">
+        <v>112</v>
+      </c>
+      <c r="G110">
+        <v>0.16</v>
+      </c>
+      <c r="H110">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111">
+        <v>-8</v>
+      </c>
+      <c r="B111">
+        <v>10</v>
+      </c>
+      <c r="C111">
+        <v>4.9098</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>250</v>
+      </c>
+      <c r="F111">
+        <v>112</v>
+      </c>
+      <c r="G111">
+        <v>0.16</v>
+      </c>
+      <c r="H111">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112">
+        <v>-7</v>
+      </c>
+      <c r="B112">
+        <v>10</v>
+      </c>
+      <c r="C112">
+        <v>5.4203</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>250</v>
+      </c>
+      <c r="F112">
+        <v>112</v>
+      </c>
+      <c r="G112">
+        <v>0.16</v>
+      </c>
+      <c r="H112">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113">
+        <v>-4</v>
+      </c>
+      <c r="B113">
+        <v>10</v>
+      </c>
+      <c r="C113">
+        <v>6.6888</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>250</v>
+      </c>
+      <c r="F113">
+        <v>112</v>
+      </c>
+      <c r="G113">
+        <v>0.16</v>
+      </c>
+      <c r="H113">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114">
+        <v>-3</v>
+      </c>
+      <c r="B114">
+        <v>10</v>
+      </c>
+      <c r="C114">
+        <v>6.8123</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>250</v>
+      </c>
+      <c r="F114">
+        <v>112</v>
+      </c>
+      <c r="G114">
+        <v>0.16</v>
+      </c>
+      <c r="H114">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115">
+        <v>0</v>
+      </c>
+      <c r="B115">
+        <v>10</v>
+      </c>
+      <c r="C115">
+        <v>4.5922</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>250</v>
+      </c>
+      <c r="F115">
+        <v>112</v>
+      </c>
+      <c r="G115">
+        <v>0.16</v>
+      </c>
+      <c r="H115">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116">
+        <v>1</v>
+      </c>
+      <c r="B116">
+        <v>10</v>
+      </c>
+      <c r="C116">
+        <v>4.6839</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>250</v>
+      </c>
+      <c r="F116">
+        <v>112</v>
+      </c>
+      <c r="G116">
+        <v>0.16</v>
+      </c>
+      <c r="H116">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117">
         <v>2</v>
       </c>
-      <c r="B99">
+      <c r="B117">
         <v>10</v>
       </c>
-      <c r="C99">
+      <c r="C117">
         <v>3.0886</v>
       </c>
-      <c r="D99">
-        <v>0</v>
-      </c>
-      <c r="E99">
-        <v>250</v>
-      </c>
-      <c r="F99">
-        <v>112</v>
-      </c>
-      <c r="G99">
-        <v>0.16</v>
-      </c>
-      <c r="H99">
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>250</v>
+      </c>
+      <c r="F117">
+        <v>112</v>
+      </c>
+      <c r="G117">
+        <v>0.16</v>
+      </c>
+      <c r="H117">
         <v>0.158</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data processed and ready to run more sims
</commit_message>
<xml_diff>
--- a/series_02/mpi_0/span_010/qsmf_output.xlsx
+++ b/series_02/mpi_0/span_010/qsmf_output.xlsx
@@ -395,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3107,13 +3107,13 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B105">
         <v>8</v>
       </c>
       <c r="C105">
-        <v>1.7325</v>
+        <v>4.2935</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -3133,13 +3133,13 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="B106">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C106">
-        <v>4.44</v>
+        <v>1.7325</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -3159,13 +3159,13 @@
     </row>
     <row r="107" spans="1:8">
       <c r="A107">
-        <v>-5</v>
+        <v>-9</v>
       </c>
       <c r="B107">
         <v>9</v>
       </c>
       <c r="C107">
-        <v>6.4409</v>
+        <v>4.44</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -3185,13 +3185,13 @@
     </row>
     <row r="108" spans="1:8">
       <c r="A108">
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="B108">
         <v>9</v>
       </c>
       <c r="C108">
-        <v>6.7729</v>
+        <v>4.9847</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -3211,13 +3211,13 @@
     </row>
     <row r="109" spans="1:8">
       <c r="A109">
-        <v>-2</v>
+        <v>-7</v>
       </c>
       <c r="B109">
         <v>9</v>
       </c>
       <c r="C109">
-        <v>6.5031</v>
+        <v>5.4923</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -3237,13 +3237,13 @@
     </row>
     <row r="110" spans="1:8">
       <c r="A110">
-        <v>-1</v>
+        <v>-6</v>
       </c>
       <c r="B110">
         <v>9</v>
       </c>
       <c r="C110">
-        <v>5.6733</v>
+        <v>5.964</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -3263,13 +3263,13 @@
     </row>
     <row r="111" spans="1:8">
       <c r="A111">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="B111">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C111">
-        <v>4.9098</v>
+        <v>6.4409</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -3289,13 +3289,13 @@
     </row>
     <row r="112" spans="1:8">
       <c r="A112">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="B112">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C112">
-        <v>5.4203</v>
+        <v>6.6913</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -3315,13 +3315,13 @@
     </row>
     <row r="113" spans="1:8">
       <c r="A113">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="B113">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C113">
-        <v>6.6888</v>
+        <v>6.7729</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -3341,13 +3341,13 @@
     </row>
     <row r="114" spans="1:8">
       <c r="A114">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="B114">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C114">
-        <v>6.8123</v>
+        <v>6.5031</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -3367,13 +3367,13 @@
     </row>
     <row r="115" spans="1:8">
       <c r="A115">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B115">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C115">
-        <v>4.5922</v>
+        <v>5.6733</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -3393,13 +3393,13 @@
     </row>
     <row r="116" spans="1:8">
       <c r="A116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B116">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C116">
-        <v>4.6839</v>
+        <v>4.6252</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -3419,27 +3419,287 @@
     </row>
     <row r="117" spans="1:8">
       <c r="A117">
+        <v>1</v>
+      </c>
+      <c r="B117">
+        <v>9</v>
+      </c>
+      <c r="C117">
+        <v>3.544</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>250</v>
+      </c>
+      <c r="F117">
+        <v>112</v>
+      </c>
+      <c r="G117">
+        <v>0.16</v>
+      </c>
+      <c r="H117">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118">
         <v>2</v>
       </c>
-      <c r="B117">
+      <c r="B118">
+        <v>9</v>
+      </c>
+      <c r="C118">
+        <v>1.4599</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <v>250</v>
+      </c>
+      <c r="F118">
+        <v>112</v>
+      </c>
+      <c r="G118">
+        <v>0.16</v>
+      </c>
+      <c r="H118">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119">
+        <v>-9</v>
+      </c>
+      <c r="B119">
         <v>10</v>
       </c>
-      <c r="C117">
+      <c r="C119">
+        <v>4.3695</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>250</v>
+      </c>
+      <c r="F119">
+        <v>112</v>
+      </c>
+      <c r="G119">
+        <v>0.16</v>
+      </c>
+      <c r="H119">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120">
+        <v>-8</v>
+      </c>
+      <c r="B120">
+        <v>10</v>
+      </c>
+      <c r="C120">
+        <v>4.9098</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <v>250</v>
+      </c>
+      <c r="F120">
+        <v>112</v>
+      </c>
+      <c r="G120">
+        <v>0.16</v>
+      </c>
+      <c r="H120">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121">
+        <v>-7</v>
+      </c>
+      <c r="B121">
+        <v>10</v>
+      </c>
+      <c r="C121">
+        <v>5.4203</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>250</v>
+      </c>
+      <c r="F121">
+        <v>112</v>
+      </c>
+      <c r="G121">
+        <v>0.16</v>
+      </c>
+      <c r="H121">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122">
+        <v>-6</v>
+      </c>
+      <c r="B122">
+        <v>10</v>
+      </c>
+      <c r="C122">
+        <v>5.9466</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>250</v>
+      </c>
+      <c r="F122">
+        <v>112</v>
+      </c>
+      <c r="G122">
+        <v>0.16</v>
+      </c>
+      <c r="H122">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123">
+        <v>-4</v>
+      </c>
+      <c r="B123">
+        <v>10</v>
+      </c>
+      <c r="C123">
+        <v>6.6888</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>250</v>
+      </c>
+      <c r="F123">
+        <v>112</v>
+      </c>
+      <c r="G123">
+        <v>0.16</v>
+      </c>
+      <c r="H123">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124">
+        <v>-3</v>
+      </c>
+      <c r="B124">
+        <v>10</v>
+      </c>
+      <c r="C124">
+        <v>6.8123</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>250</v>
+      </c>
+      <c r="F124">
+        <v>112</v>
+      </c>
+      <c r="G124">
+        <v>0.16</v>
+      </c>
+      <c r="H124">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125">
+        <v>0</v>
+      </c>
+      <c r="B125">
+        <v>10</v>
+      </c>
+      <c r="C125">
+        <v>4.5922</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>250</v>
+      </c>
+      <c r="F125">
+        <v>112</v>
+      </c>
+      <c r="G125">
+        <v>0.16</v>
+      </c>
+      <c r="H125">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126">
+        <v>10</v>
+      </c>
+      <c r="C126">
+        <v>4.6839</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>250</v>
+      </c>
+      <c r="F126">
+        <v>112</v>
+      </c>
+      <c r="G126">
+        <v>0.16</v>
+      </c>
+      <c r="H126">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127">
+        <v>2</v>
+      </c>
+      <c r="B127">
+        <v>10</v>
+      </c>
+      <c r="C127">
         <v>3.0886</v>
       </c>
-      <c r="D117">
-        <v>0</v>
-      </c>
-      <c r="E117">
-        <v>250</v>
-      </c>
-      <c r="F117">
-        <v>112</v>
-      </c>
-      <c r="G117">
-        <v>0.16</v>
-      </c>
-      <c r="H117">
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>250</v>
+      </c>
+      <c r="F127">
+        <v>112</v>
+      </c>
+      <c r="G127">
+        <v>0.16</v>
+      </c>
+      <c r="H127">
         <v>0.158</v>
       </c>
     </row>

</xml_diff>

<commit_message>
check for fully complete sets
</commit_message>
<xml_diff>
--- a/series_02/mpi_0/span_010/qsmf_output.xlsx
+++ b/series_02/mpi_0/span_010/qsmf_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Laser Power (dBm)</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Q (dB)</t>
+  </si>
+  <si>
+    <t>Span (km)</t>
   </si>
   <si>
     <t>Compensation (%)</t>
@@ -395,13 +398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +429,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>-9</v>
       </c>
@@ -437,23 +443,23 @@
       <c r="C2">
         <v>4.8209</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
       <c r="E2">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G2">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H2">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I2">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>-8</v>
       </c>
@@ -463,23 +469,23 @@
       <c r="C3">
         <v>5.5555</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
       <c r="E3">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G3">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H3">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I3">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>-7</v>
       </c>
@@ -489,23 +495,23 @@
       <c r="C4">
         <v>6.1533</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G4">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H4">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I4">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>-6</v>
       </c>
@@ -515,23 +521,23 @@
       <c r="C5">
         <v>6.3825</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
       <c r="E5">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G5">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H5">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I5">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>-5</v>
       </c>
@@ -541,23 +547,23 @@
       <c r="C6">
         <v>6.2083</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
       <c r="E6">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G6">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H6">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I6">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>-4</v>
       </c>
@@ -567,23 +573,23 @@
       <c r="C7">
         <v>5.4519</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
       <c r="E7">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G7">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H7">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I7">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>-3</v>
       </c>
@@ -593,23 +599,23 @@
       <c r="C8">
         <v>4.6411</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
       <c r="E8">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G8">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H8">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I8">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>-2</v>
       </c>
@@ -619,23 +625,23 @@
       <c r="C9">
         <v>2.9553</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
       <c r="E9">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G9">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H9">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I9">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>-1</v>
       </c>
@@ -645,23 +651,23 @@
       <c r="C10">
         <v>1.8352</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
       <c r="E10">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G10">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H10">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I10">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>0</v>
       </c>
@@ -671,23 +677,23 @@
       <c r="C11">
         <v>0.5206499999999999</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G11">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H11">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I11">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>1</v>
       </c>
@@ -697,23 +703,23 @@
       <c r="C12">
         <v>-2.3361</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
       <c r="E12">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G12">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H12">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I12">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>2</v>
       </c>
@@ -723,23 +729,23 @@
       <c r="C13">
         <v>-4.4091</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
       <c r="E13">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G13">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H13">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I13">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>-9</v>
       </c>
@@ -749,23 +755,23 @@
       <c r="C14">
         <v>4.8502</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
       <c r="E14">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G14">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H14">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I14">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>-8</v>
       </c>
@@ -775,23 +781,23 @@
       <c r="C15">
         <v>5.5923</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
       <c r="E15">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G15">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H15">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I15">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>-7</v>
       </c>
@@ -801,23 +807,23 @@
       <c r="C16">
         <v>6.1112</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
       <c r="E16">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G16">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H16">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I16">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>-6</v>
       </c>
@@ -827,23 +833,23 @@
       <c r="C17">
         <v>6.4461</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
       <c r="E17">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G17">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H17">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I17">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>-5</v>
       </c>
@@ -853,23 +859,23 @@
       <c r="C18">
         <v>6.4789</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
       <c r="E18">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G18">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H18">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I18">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>-4</v>
       </c>
@@ -879,23 +885,23 @@
       <c r="C19">
         <v>5.7639</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
       <c r="E19">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G19">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H19">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I19">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>-3</v>
       </c>
@@ -905,23 +911,23 @@
       <c r="C20">
         <v>5.1653</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
       <c r="E20">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G20">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H20">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I20">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>-2</v>
       </c>
@@ -931,23 +937,23 @@
       <c r="C21">
         <v>4.3699</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
       <c r="E21">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G21">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H21">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I21">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>-1</v>
       </c>
@@ -957,23 +963,23 @@
       <c r="C22">
         <v>2.1476</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
       <c r="E22">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G22">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H22">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I22">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>0</v>
       </c>
@@ -983,23 +989,23 @@
       <c r="C23">
         <v>0.31632</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
       <c r="E23">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G23">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H23">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I23">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1009,23 +1015,23 @@
       <c r="C24">
         <v>-2.5114</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
       <c r="E24">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G24">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H24">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I24">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1035,23 +1041,23 @@
       <c r="C25">
         <v>-4.0578</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
       <c r="E25">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G25">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H25">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I25">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>-9</v>
       </c>
@@ -1061,23 +1067,23 @@
       <c r="C26">
         <v>4.8874</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
       <c r="E26">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G26">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H26">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I26">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>-8</v>
       </c>
@@ -1087,23 +1093,23 @@
       <c r="C27">
         <v>5.5951</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
       <c r="E27">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G27">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H27">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I27">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>-7</v>
       </c>
@@ -1113,23 +1119,23 @@
       <c r="C28">
         <v>6.1807</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
       <c r="E28">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G28">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H28">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I28">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>-6</v>
       </c>
@@ -1139,23 +1145,23 @@
       <c r="C29">
         <v>6.6013</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
       <c r="E29">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G29">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H29">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I29">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>-5</v>
       </c>
@@ -1165,23 +1171,23 @@
       <c r="C30">
         <v>6.559</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
       <c r="E30">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G30">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H30">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I30">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>-4</v>
       </c>
@@ -1191,23 +1197,23 @@
       <c r="C31">
         <v>6.4343</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
       <c r="E31">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G31">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H31">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I31">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>-3</v>
       </c>
@@ -1217,23 +1223,23 @@
       <c r="C32">
         <v>4.407</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
       <c r="E32">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G32">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H32">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I32">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>-2</v>
       </c>
@@ -1243,23 +1249,23 @@
       <c r="C33">
         <v>4.8755</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
       <c r="E33">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G33">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H33">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I33">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>-1</v>
       </c>
@@ -1269,23 +1275,23 @@
       <c r="C34">
         <v>2.568</v>
       </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
       <c r="E34">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G34">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H34">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I34">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>0</v>
       </c>
@@ -1295,23 +1301,23 @@
       <c r="C35">
         <v>0.87279</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
       <c r="E35">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G35">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H35">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I35">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1321,23 +1327,23 @@
       <c r="C36">
         <v>-1.5232</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
       <c r="E36">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G36">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H36">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I36">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1347,23 +1353,23 @@
       <c r="C37">
         <v>-2.3355</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
       <c r="E37">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G37">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H37">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I37">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>-9</v>
       </c>
@@ -1373,23 +1379,23 @@
       <c r="C38">
         <v>4.8025</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
       <c r="E38">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G38">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H38">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I38">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>-8</v>
       </c>
@@ -1399,23 +1405,23 @@
       <c r="C39">
         <v>5.4323</v>
       </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
       <c r="E39">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G39">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H39">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I39">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>-7</v>
       </c>
@@ -1425,23 +1431,23 @@
       <c r="C40">
         <v>6.0363</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
       <c r="E40">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G40">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H40">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I40">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>-6</v>
       </c>
@@ -1451,23 +1457,23 @@
       <c r="C41">
         <v>6.438</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
       <c r="E41">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G41">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H41">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I41">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>-5</v>
       </c>
@@ -1477,23 +1483,23 @@
       <c r="C42">
         <v>6.573</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
       <c r="E42">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G42">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H42">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I42">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>-4</v>
       </c>
@@ -1503,23 +1509,23 @@
       <c r="C43">
         <v>6.4321</v>
       </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
       <c r="E43">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G43">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H43">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I43">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>-3</v>
       </c>
@@ -1529,23 +1535,23 @@
       <c r="C44">
         <v>6.0446</v>
       </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
       <c r="E44">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G44">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H44">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I44">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>-2</v>
       </c>
@@ -1555,23 +1561,23 @@
       <c r="C45">
         <v>4.847</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
       <c r="E45">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G45">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H45">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I45">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>-1</v>
       </c>
@@ -1581,23 +1587,23 @@
       <c r="C46">
         <v>3.123</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
       <c r="E46">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G46">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H46">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I46">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>0</v>
       </c>
@@ -1607,23 +1613,23 @@
       <c r="C47">
         <v>1.6808</v>
       </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
       <c r="E47">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G47">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H47">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I47">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>1</v>
       </c>
@@ -1633,23 +1639,23 @@
       <c r="C48">
         <v>-0.7821600000000001</v>
       </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
       <c r="E48">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G48">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H48">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I48">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1659,23 +1665,23 @@
       <c r="C49">
         <v>-3.0472</v>
       </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
       <c r="E49">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G49">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H49">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I49">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50">
         <v>-9</v>
       </c>
@@ -1685,23 +1691,23 @@
       <c r="C50">
         <v>4.7523</v>
       </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
       <c r="E50">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G50">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H50">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I50">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51">
         <v>-8</v>
       </c>
@@ -1711,23 +1717,23 @@
       <c r="C51">
         <v>5.4371</v>
       </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
       <c r="E51">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G51">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H51">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I51">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52">
         <v>-7</v>
       </c>
@@ -1737,23 +1743,23 @@
       <c r="C52">
         <v>6.0223</v>
       </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
       <c r="E52">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G52">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H52">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I52">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53">
         <v>-6</v>
       </c>
@@ -1763,23 +1769,23 @@
       <c r="C53">
         <v>6.4797</v>
       </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
       <c r="E53">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F53">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G53">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H53">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I53">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54">
         <v>-5</v>
       </c>
@@ -1789,23 +1795,23 @@
       <c r="C54">
         <v>6.6823</v>
       </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
       <c r="E54">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G54">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H54">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I54">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55">
         <v>-4</v>
       </c>
@@ -1815,23 +1821,23 @@
       <c r="C55">
         <v>6.584</v>
       </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
       <c r="E55">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G55">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H55">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I55">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56">
         <v>-3</v>
       </c>
@@ -1841,23 +1847,23 @@
       <c r="C56">
         <v>5.7954</v>
       </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
       <c r="E56">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G56">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H56">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I56">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57">
         <v>-2</v>
       </c>
@@ -1867,23 +1873,23 @@
       <c r="C57">
         <v>5.0279</v>
       </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
       <c r="E57">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F57">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G57">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H57">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I57">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58">
         <v>-1</v>
       </c>
@@ -1893,23 +1899,23 @@
       <c r="C58">
         <v>4.0717</v>
       </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
       <c r="E58">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G58">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H58">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I58">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59">
         <v>0</v>
       </c>
@@ -1919,23 +1925,23 @@
       <c r="C59">
         <v>2.3168</v>
       </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
       <c r="E59">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G59">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H59">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I59">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1945,23 +1951,23 @@
       <c r="C60">
         <v>0.19125</v>
       </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
       <c r="E60">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F60">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G60">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H60">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I60">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61">
         <v>2</v>
       </c>
@@ -1971,23 +1977,23 @@
       <c r="C61">
         <v>-1.9133</v>
       </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
       <c r="E61">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F61">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G61">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H61">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I61">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62">
         <v>-9</v>
       </c>
@@ -1997,23 +2003,23 @@
       <c r="C62">
         <v>4.6579</v>
       </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
       <c r="E62">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G62">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H62">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I62">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63">
         <v>-8</v>
       </c>
@@ -2023,23 +2029,23 @@
       <c r="C63">
         <v>5.3594</v>
       </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
       <c r="E63">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F63">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G63">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H63">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I63">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64">
         <v>-7</v>
       </c>
@@ -2049,23 +2055,23 @@
       <c r="C64">
         <v>5.8256</v>
       </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
       <c r="E64">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F64">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G64">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H64">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I64">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65">
         <v>-6</v>
       </c>
@@ -2075,23 +2081,23 @@
       <c r="C65">
         <v>6.3104</v>
       </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
       <c r="E65">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F65">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G65">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H65">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I65">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66">
         <v>-5</v>
       </c>
@@ -2101,23 +2107,23 @@
       <c r="C66">
         <v>6.7243</v>
       </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
       <c r="E66">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G66">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H66">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I66">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67">
         <v>-4</v>
       </c>
@@ -2127,23 +2133,23 @@
       <c r="C67">
         <v>6.6547</v>
       </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
       <c r="E67">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G67">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H67">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I67">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68">
         <v>-3</v>
       </c>
@@ -2153,23 +2159,23 @@
       <c r="C68">
         <v>6.2873</v>
       </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
       <c r="E68">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F68">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G68">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H68">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I68">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69">
         <v>-2</v>
       </c>
@@ -2179,23 +2185,23 @@
       <c r="C69">
         <v>5.3266</v>
       </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
       <c r="E69">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F69">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G69">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H69">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I69">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70">
         <v>-1</v>
       </c>
@@ -2205,23 +2211,23 @@
       <c r="C70">
         <v>4.4445</v>
       </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
       <c r="E70">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F70">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G70">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H70">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I70">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71">
         <v>0</v>
       </c>
@@ -2231,23 +2237,23 @@
       <c r="C71">
         <v>2.6343</v>
       </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
       <c r="E71">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G71">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H71">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I71">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72">
         <v>1</v>
       </c>
@@ -2257,23 +2263,23 @@
       <c r="C72">
         <v>-0.019673</v>
       </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
       <c r="E72">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G72">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H72">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I72">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73">
         <v>2</v>
       </c>
@@ -2283,23 +2289,23 @@
       <c r="C73">
         <v>-1.4611</v>
       </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
       <c r="E73">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F73">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G73">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H73">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I73">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74">
         <v>-9</v>
       </c>
@@ -2309,23 +2315,23 @@
       <c r="C74">
         <v>4.6033</v>
       </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
       <c r="E74">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G74">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H74">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I74">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75">
         <v>-8</v>
       </c>
@@ -2335,23 +2341,23 @@
       <c r="C75">
         <v>5.2784</v>
       </c>
-      <c r="D75">
-        <v>0</v>
-      </c>
       <c r="E75">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F75">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G75">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H75">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I75">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76">
         <v>-7</v>
       </c>
@@ -2361,23 +2367,23 @@
       <c r="C76">
         <v>5.8279</v>
       </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
       <c r="E76">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F76">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G76">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H76">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I76">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77">
         <v>-6</v>
       </c>
@@ -2387,23 +2393,23 @@
       <c r="C77">
         <v>6.3401</v>
       </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
       <c r="E77">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F77">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G77">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H77">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I77">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78">
         <v>-5</v>
       </c>
@@ -2413,23 +2419,23 @@
       <c r="C78">
         <v>6.6346</v>
       </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
       <c r="E78">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F78">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G78">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H78">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I78">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79">
         <v>-4</v>
       </c>
@@ -2439,23 +2445,23 @@
       <c r="C79">
         <v>6.7814</v>
       </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
       <c r="E79">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F79">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G79">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H79">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I79">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80">
         <v>-3</v>
       </c>
@@ -2465,23 +2471,23 @@
       <c r="C80">
         <v>6.4291</v>
       </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
       <c r="E80">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G80">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H80">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I80">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81">
         <v>-2</v>
       </c>
@@ -2491,23 +2497,23 @@
       <c r="C81">
         <v>5.3739</v>
       </c>
-      <c r="D81">
-        <v>0</v>
-      </c>
       <c r="E81">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F81">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G81">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H81">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I81">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
       <c r="A82">
         <v>-1</v>
       </c>
@@ -2517,23 +2523,23 @@
       <c r="C82">
         <v>5.1433</v>
       </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
       <c r="E82">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F82">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G82">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H82">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I82">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83">
         <v>0</v>
       </c>
@@ -2543,23 +2549,23 @@
       <c r="C83">
         <v>3.2795</v>
       </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
       <c r="E83">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G83">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H83">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I83">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84">
         <v>1</v>
       </c>
@@ -2569,23 +2575,23 @@
       <c r="C84">
         <v>0.64904</v>
       </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
       <c r="E84">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G84">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H84">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I84">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85">
         <v>2</v>
       </c>
@@ -2595,23 +2601,23 @@
       <c r="C85">
         <v>-2.2381</v>
       </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
       <c r="E85">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F85">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G85">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H85">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I85">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86">
         <v>-9</v>
       </c>
@@ -2621,23 +2627,23 @@
       <c r="C86">
         <v>4.5494</v>
       </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
       <c r="E86">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F86">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G86">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H86">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I86">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87">
         <v>-8</v>
       </c>
@@ -2647,23 +2653,23 @@
       <c r="C87">
         <v>5.1638</v>
       </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
       <c r="E87">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F87">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G87">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H87">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I87">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88">
         <v>-7</v>
       </c>
@@ -2673,23 +2679,23 @@
       <c r="C88">
         <v>5.7085</v>
       </c>
-      <c r="D88">
-        <v>0</v>
-      </c>
       <c r="E88">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F88">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G88">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H88">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I88">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89">
         <v>-6</v>
       </c>
@@ -2699,23 +2705,23 @@
       <c r="C89">
         <v>6.2424</v>
       </c>
-      <c r="D89">
-        <v>0</v>
-      </c>
       <c r="E89">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G89">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H89">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I89">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90">
         <v>-5</v>
       </c>
@@ -2725,23 +2731,23 @@
       <c r="C90">
         <v>6.5467</v>
       </c>
-      <c r="D90">
-        <v>0</v>
-      </c>
       <c r="E90">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G90">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H90">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I90">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91">
         <v>-4</v>
       </c>
@@ -2751,23 +2757,23 @@
       <c r="C91">
         <v>6.7052</v>
       </c>
-      <c r="D91">
-        <v>0</v>
-      </c>
       <c r="E91">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G91">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H91">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I91">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92">
         <v>-3</v>
       </c>
@@ -2777,23 +2783,23 @@
       <c r="C92">
         <v>6.5723</v>
       </c>
-      <c r="D92">
-        <v>0</v>
-      </c>
       <c r="E92">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F92">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G92">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H92">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I92">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93">
         <v>-2</v>
       </c>
@@ -2803,23 +2809,23 @@
       <c r="C93">
         <v>5.7703</v>
       </c>
-      <c r="D93">
-        <v>0</v>
-      </c>
       <c r="E93">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F93">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G93">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H93">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I93">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94">
         <v>-1</v>
       </c>
@@ -2829,23 +2835,23 @@
       <c r="C94">
         <v>5.1051</v>
       </c>
-      <c r="D94">
-        <v>0</v>
-      </c>
       <c r="E94">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G94">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H94">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I94">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95">
         <v>0</v>
       </c>
@@ -2855,23 +2861,23 @@
       <c r="C95">
         <v>3.7594</v>
       </c>
-      <c r="D95">
-        <v>0</v>
-      </c>
       <c r="E95">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F95">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G95">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H95">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I95">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96">
         <v>1</v>
       </c>
@@ -2881,23 +2887,23 @@
       <c r="C96">
         <v>2.2049</v>
       </c>
-      <c r="D96">
-        <v>0</v>
-      </c>
       <c r="E96">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F96">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G96">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H96">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I96">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97">
         <v>2</v>
       </c>
@@ -2907,23 +2913,23 @@
       <c r="C97">
         <v>-0.62087</v>
       </c>
-      <c r="D97">
-        <v>0</v>
-      </c>
       <c r="E97">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F97">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G97">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H97">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I97">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98">
         <v>-9</v>
       </c>
@@ -2933,23 +2939,23 @@
       <c r="C98">
         <v>4.5279</v>
       </c>
-      <c r="D98">
-        <v>0</v>
-      </c>
       <c r="E98">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G98">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H98">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I98">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
       <c r="A99">
         <v>-8</v>
       </c>
@@ -2959,23 +2965,23 @@
       <c r="C99">
         <v>5.0744</v>
       </c>
-      <c r="D99">
-        <v>0</v>
-      </c>
       <c r="E99">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F99">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G99">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H99">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I99">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100">
         <v>-7</v>
       </c>
@@ -2985,23 +2991,23 @@
       <c r="C100">
         <v>5.5962</v>
       </c>
-      <c r="D100">
-        <v>0</v>
-      </c>
       <c r="E100">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G100">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H100">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I100">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
       <c r="A101">
         <v>-6</v>
       </c>
@@ -3011,23 +3017,23 @@
       <c r="C101">
         <v>6.1046</v>
       </c>
-      <c r="D101">
-        <v>0</v>
-      </c>
       <c r="E101">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F101">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G101">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H101">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I101">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
       <c r="A102">
         <v>-5</v>
       </c>
@@ -3037,23 +3043,23 @@
       <c r="C102">
         <v>6.5001</v>
       </c>
-      <c r="D102">
-        <v>0</v>
-      </c>
       <c r="E102">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F102">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G102">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H102">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I102">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
       <c r="A103">
         <v>-4</v>
       </c>
@@ -3063,23 +3069,23 @@
       <c r="C103">
         <v>6.8227</v>
       </c>
-      <c r="D103">
-        <v>0</v>
-      </c>
       <c r="E103">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F103">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G103">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H103">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I103">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
       <c r="A104">
         <v>-3</v>
       </c>
@@ -3089,23 +3095,23 @@
       <c r="C104">
         <v>6.7209</v>
       </c>
-      <c r="D104">
-        <v>0</v>
-      </c>
       <c r="E104">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F104">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G104">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H104">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I104">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
       <c r="A105">
         <v>-2</v>
       </c>
@@ -3115,23 +3121,23 @@
       <c r="C105">
         <v>6.3868</v>
       </c>
-      <c r="D105">
-        <v>0</v>
-      </c>
       <c r="E105">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F105">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G105">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H105">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I105">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
       <c r="A106">
         <v>-1</v>
       </c>
@@ -3141,23 +3147,23 @@
       <c r="C106">
         <v>5.8578</v>
       </c>
-      <c r="D106">
-        <v>0</v>
-      </c>
       <c r="E106">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F106">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G106">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H106">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I106">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
       <c r="A107">
         <v>0</v>
       </c>
@@ -3167,23 +3173,23 @@
       <c r="C107">
         <v>4.2935</v>
       </c>
-      <c r="D107">
-        <v>0</v>
-      </c>
       <c r="E107">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F107">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G107">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H107">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I107">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
       <c r="A108">
         <v>1</v>
       </c>
@@ -3193,23 +3199,23 @@
       <c r="C108">
         <v>1.7325</v>
       </c>
-      <c r="D108">
-        <v>0</v>
-      </c>
       <c r="E108">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F108">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G108">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H108">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I108">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
       <c r="A109">
         <v>2</v>
       </c>
@@ -3219,23 +3225,23 @@
       <c r="C109">
         <v>0.54023</v>
       </c>
-      <c r="D109">
-        <v>0</v>
-      </c>
       <c r="E109">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G109">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H109">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I109">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
       <c r="A110">
         <v>-9</v>
       </c>
@@ -3245,23 +3251,23 @@
       <c r="C110">
         <v>4.44</v>
       </c>
-      <c r="D110">
-        <v>0</v>
-      </c>
       <c r="E110">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F110">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G110">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H110">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I110">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
       <c r="A111">
         <v>-8</v>
       </c>
@@ -3271,23 +3277,23 @@
       <c r="C111">
         <v>4.9847</v>
       </c>
-      <c r="D111">
-        <v>0</v>
-      </c>
       <c r="E111">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F111">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G111">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H111">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I111">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
       <c r="A112">
         <v>-7</v>
       </c>
@@ -3297,23 +3303,23 @@
       <c r="C112">
         <v>5.4923</v>
       </c>
-      <c r="D112">
-        <v>0</v>
-      </c>
       <c r="E112">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F112">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G112">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H112">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I112">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
       <c r="A113">
         <v>-6</v>
       </c>
@@ -3323,23 +3329,23 @@
       <c r="C113">
         <v>5.964</v>
       </c>
-      <c r="D113">
-        <v>0</v>
-      </c>
       <c r="E113">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F113">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G113">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H113">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I113">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
       <c r="A114">
         <v>-5</v>
       </c>
@@ -3349,23 +3355,23 @@
       <c r="C114">
         <v>6.4409</v>
       </c>
-      <c r="D114">
-        <v>0</v>
-      </c>
       <c r="E114">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F114">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G114">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H114">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I114">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
       <c r="A115">
         <v>-4</v>
       </c>
@@ -3375,23 +3381,23 @@
       <c r="C115">
         <v>6.6913</v>
       </c>
-      <c r="D115">
-        <v>0</v>
-      </c>
       <c r="E115">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F115">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G115">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H115">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I115">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
       <c r="A116">
         <v>-3</v>
       </c>
@@ -3401,23 +3407,23 @@
       <c r="C116">
         <v>6.7729</v>
       </c>
-      <c r="D116">
-        <v>0</v>
-      </c>
       <c r="E116">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F116">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G116">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H116">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I116">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
       <c r="A117">
         <v>-2</v>
       </c>
@@ -3427,23 +3433,23 @@
       <c r="C117">
         <v>6.5031</v>
       </c>
-      <c r="D117">
-        <v>0</v>
-      </c>
       <c r="E117">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F117">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G117">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H117">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I117">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
       <c r="A118">
         <v>-1</v>
       </c>
@@ -3453,23 +3459,23 @@
       <c r="C118">
         <v>5.6733</v>
       </c>
-      <c r="D118">
-        <v>0</v>
-      </c>
       <c r="E118">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F118">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G118">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H118">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I118">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
       <c r="A119">
         <v>0</v>
       </c>
@@ -3479,23 +3485,23 @@
       <c r="C119">
         <v>4.6252</v>
       </c>
-      <c r="D119">
-        <v>0</v>
-      </c>
       <c r="E119">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F119">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G119">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H119">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I119">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
       <c r="A120">
         <v>1</v>
       </c>
@@ -3505,23 +3511,23 @@
       <c r="C120">
         <v>3.544</v>
       </c>
-      <c r="D120">
-        <v>0</v>
-      </c>
       <c r="E120">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F120">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G120">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H120">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I120">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
       <c r="A121">
         <v>2</v>
       </c>
@@ -3531,23 +3537,23 @@
       <c r="C121">
         <v>1.4599</v>
       </c>
-      <c r="D121">
-        <v>0</v>
-      </c>
       <c r="E121">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F121">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G121">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H121">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I121">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
       <c r="A122">
         <v>-9</v>
       </c>
@@ -3557,23 +3563,23 @@
       <c r="C122">
         <v>4.3695</v>
       </c>
-      <c r="D122">
-        <v>0</v>
-      </c>
       <c r="E122">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F122">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G122">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H122">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I122">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
       <c r="A123">
         <v>-8</v>
       </c>
@@ -3583,23 +3589,23 @@
       <c r="C123">
         <v>4.9098</v>
       </c>
-      <c r="D123">
-        <v>0</v>
-      </c>
       <c r="E123">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F123">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G123">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H123">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I123">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
       <c r="A124">
         <v>-7</v>
       </c>
@@ -3609,23 +3615,23 @@
       <c r="C124">
         <v>5.4203</v>
       </c>
-      <c r="D124">
-        <v>0</v>
-      </c>
       <c r="E124">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F124">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G124">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H124">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I124">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
       <c r="A125">
         <v>-6</v>
       </c>
@@ -3635,23 +3641,23 @@
       <c r="C125">
         <v>5.9466</v>
       </c>
-      <c r="D125">
-        <v>0</v>
-      </c>
       <c r="E125">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F125">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G125">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H125">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I125">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
       <c r="A126">
         <v>-5</v>
       </c>
@@ -3661,23 +3667,23 @@
       <c r="C126">
         <v>6.2817</v>
       </c>
-      <c r="D126">
-        <v>0</v>
-      </c>
       <c r="E126">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F126">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G126">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H126">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I126">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
       <c r="A127">
         <v>-4</v>
       </c>
@@ -3687,23 +3693,23 @@
       <c r="C127">
         <v>6.6888</v>
       </c>
-      <c r="D127">
-        <v>0</v>
-      </c>
       <c r="E127">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F127">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G127">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H127">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I127">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
       <c r="A128">
         <v>-3</v>
       </c>
@@ -3713,23 +3719,23 @@
       <c r="C128">
         <v>6.8123</v>
       </c>
-      <c r="D128">
-        <v>0</v>
-      </c>
       <c r="E128">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F128">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G128">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H128">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I128">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
       <c r="A129">
         <v>-2</v>
       </c>
@@ -3739,23 +3745,23 @@
       <c r="C129">
         <v>6.6685</v>
       </c>
-      <c r="D129">
-        <v>0</v>
-      </c>
       <c r="E129">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F129">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G129">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H129">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I129">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
       <c r="A130">
         <v>-1</v>
       </c>
@@ -3765,23 +3771,23 @@
       <c r="C130">
         <v>6.337999999999999</v>
       </c>
-      <c r="D130">
-        <v>0</v>
-      </c>
       <c r="E130">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F130">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G130">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H130">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I130">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
       <c r="A131">
         <v>0</v>
       </c>
@@ -3791,23 +3797,23 @@
       <c r="C131">
         <v>4.5922</v>
       </c>
-      <c r="D131">
-        <v>0</v>
-      </c>
       <c r="E131">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F131">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G131">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H131">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I131">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
       <c r="A132">
         <v>1</v>
       </c>
@@ -3817,23 +3823,23 @@
       <c r="C132">
         <v>4.6839</v>
       </c>
-      <c r="D132">
-        <v>0</v>
-      </c>
       <c r="E132">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F132">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G132">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H132">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8">
+        <v>0.16</v>
+      </c>
+      <c r="I132">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
       <c r="A133">
         <v>2</v>
       </c>
@@ -3843,19 +3849,19 @@
       <c r="C133">
         <v>3.0886</v>
       </c>
-      <c r="D133">
-        <v>0</v>
-      </c>
       <c r="E133">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F133">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G133">
-        <v>0.16</v>
+        <v>112</v>
       </c>
       <c r="H133">
+        <v>0.16</v>
+      </c>
+      <c r="I133">
         <v>0.158</v>
       </c>
     </row>

</xml_diff>